<commit_message>
adding example xlsx file
</commit_message>
<xml_diff>
--- a/deltagare.xlsx
+++ b/deltagare.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>pvilje</t>
-  </si>
-  <si>
     <t>name 1</t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>name 18</t>
+  </si>
+  <si>
+    <t>name 16</t>
   </si>
 </sst>
 </file>
@@ -409,102 +409,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A2:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continued work on accepting previous results as start point.
</commit_message>
<xml_diff>
--- a/deltagare.xlsx
+++ b/deltagare.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>name 1</t>
   </si>
@@ -68,12 +68,48 @@
   </si>
   <si>
     <t>name 16</t>
+  </si>
+  <si>
+    <t>name 19</t>
+  </si>
+  <si>
+    <t>name 20</t>
+  </si>
+  <si>
+    <t>name 21</t>
+  </si>
+  <si>
+    <t>name 22</t>
+  </si>
+  <si>
+    <t>name 23</t>
+  </si>
+  <si>
+    <t>name 24</t>
+  </si>
+  <si>
+    <t>name 25</t>
+  </si>
+  <si>
+    <t>name 26</t>
+  </si>
+  <si>
+    <t>name 27</t>
+  </si>
+  <si>
+    <t>name 28</t>
+  </si>
+  <si>
+    <t>name 29</t>
+  </si>
+  <si>
+    <t>name 30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,7 +159,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -198,6 +234,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -233,6 +286,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A19"/>
+  <dimension ref="A2:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A19" sqref="A19:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,6 +577,66 @@
         <v>16</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>